<commit_message>
Popravljeni izpis v Excel in dodan primer za domačo nalogo.
</commit_message>
<xml_diff>
--- a/matlab/voyage_plan.xlsx
+++ b/matlab/voyage_plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Sandro\Data\Documents\02_FPP\03_classes\1.stopnja\Oceanska_Navigacija\lectures\agrm\02_voyage_plan\examples\ocean_navigation\matlab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Data\Documents\02_FPP\03_classes\1.stopnja\Oceanska_Navigacija\lectures\agrm\02_voyage_plan\examples\ocean_navigation\matlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="RL-GC data" sheetId="1" r:id="rId1"/>
     <sheet name="ETA calculator" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
     <numFmt numFmtId="165" formatCode="hh:mm:ss;@"/>
@@ -117,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -132,18 +132,239 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -157,6 +378,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,637 +695,699 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2" s="1"/>
+      <c r="D2" s="30"/>
       <c r="F2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G2" s="30"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
+      <c r="D3" s="31"/>
       <c r="F3" s="1"/>
+      <c r="G3" s="31"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
+      <c r="D4" s="32"/>
       <c r="F4" s="1"/>
+      <c r="G4" s="32"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
+      <c r="D5" s="33"/>
       <c r="F5" s="1"/>
+      <c r="G5" s="33"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
+      <c r="D6" s="34"/>
       <c r="F6" s="1"/>
+      <c r="G6" s="34"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
+      <c r="D7" s="35"/>
       <c r="F7" s="1"/>
+      <c r="G7" s="35"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
+      <c r="D8" s="36"/>
       <c r="F8" s="1"/>
+      <c r="G8" s="36"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
+      <c r="D9" s="37"/>
       <c r="F9" s="1"/>
+      <c r="G9" s="37"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
+      <c r="D10" s="38"/>
       <c r="F10" s="1"/>
+      <c r="G10" s="38"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
+      <c r="D11" s="39"/>
       <c r="F11" s="1"/>
+      <c r="G11" s="39"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
+      <c r="D12" s="40"/>
       <c r="F12" s="1"/>
+      <c r="G12" s="40"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
+      <c r="D13" s="41"/>
       <c r="F13" s="1"/>
+      <c r="G13" s="41"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
+      <c r="D14" s="10"/>
       <c r="F14" s="1"/>
+      <c r="G14" s="10"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
+      <c r="D15" s="11"/>
       <c r="F15" s="1"/>
+      <c r="G15" s="11"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
+      <c r="D16" s="12"/>
       <c r="F16" s="1"/>
+      <c r="G16" s="12"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
+      <c r="D17" s="13"/>
       <c r="F17" s="1"/>
+      <c r="G17" s="13"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
+      <c r="D18" s="14"/>
       <c r="F18" s="1"/>
+      <c r="G18" s="14"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
+      <c r="D19" s="15"/>
       <c r="F19" s="1"/>
+      <c r="G19" s="15"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
+      <c r="D20" s="16"/>
       <c r="F20" s="1"/>
+      <c r="G20" s="16"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
+      <c r="D21" s="17"/>
       <c r="F21" s="1"/>
+      <c r="G21" s="17"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
+      <c r="D22" s="18"/>
       <c r="F22" s="1"/>
+      <c r="G22" s="18"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
+      <c r="D23" s="19"/>
       <c r="F23" s="1"/>
+      <c r="G23" s="19"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
+      <c r="D24" s="20"/>
       <c r="F24" s="1"/>
+      <c r="G24" s="20"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
+      <c r="D25" s="21"/>
       <c r="F25" s="1"/>
+      <c r="G25" s="21"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
+      <c r="D26" s="22"/>
       <c r="F26" s="1"/>
+      <c r="G26" s="22"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
+      <c r="D27" s="23"/>
       <c r="F27" s="1"/>
+      <c r="G27" s="23"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
+      <c r="D28" s="24"/>
       <c r="F28" s="1"/>
+      <c r="G28" s="24"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
+      <c r="D29" s="25"/>
       <c r="F29" s="1"/>
+      <c r="G29" s="25"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
+      <c r="D30" s="26"/>
       <c r="F30" s="1"/>
+      <c r="G30" s="26"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C31" s="1"/>
+      <c r="D31" s="27"/>
       <c r="F31" s="1"/>
+      <c r="G31" s="27"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C32" s="1"/>
+      <c r="D32" s="28"/>
       <c r="F32" s="1"/>
+      <c r="G32" s="28"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
+      <c r="D33" s="29"/>
       <c r="F33" s="1"/>
+      <c r="G33" s="29"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C34" s="1"/>
       <c r="F34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C35" s="1"/>
       <c r="F35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C36" s="1"/>
       <c r="F36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C37" s="1"/>
       <c r="F37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C38" s="1"/>
       <c r="F38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C39" s="1"/>
       <c r="F39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C40" s="1"/>
       <c r="F40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C41" s="1"/>
       <c r="F41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C42" s="1"/>
       <c r="F42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C43" s="1"/>
       <c r="F43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C44" s="1"/>
       <c r="F44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C45" s="1"/>
       <c r="F45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C46" s="1"/>
       <c r="F46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C47" s="1"/>
       <c r="F47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C48" s="1"/>
       <c r="F48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C49" s="1"/>
       <c r="F49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C50" s="1"/>
       <c r="F50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C51" s="1"/>
       <c r="F51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C52" s="1"/>
       <c r="F52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C53" s="1"/>
       <c r="F53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C54" s="1"/>
       <c r="F54" s="1"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C55" s="1"/>
       <c r="F55" s="1"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C56" s="1"/>
       <c r="F56" s="1"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C57" s="1"/>
       <c r="F57" s="1"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C58" s="1"/>
       <c r="F58" s="1"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C59" s="1"/>
       <c r="F59" s="1"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C60" s="1"/>
       <c r="F60" s="1"/>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C61" s="1"/>
       <c r="F61" s="1"/>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C62" s="1"/>
       <c r="F62" s="1"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C63" s="1"/>
       <c r="F63" s="1"/>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C64" s="1"/>
       <c r="F64" s="1"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C65" s="1"/>
       <c r="F65" s="1"/>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C66" s="1"/>
       <c r="F66" s="1"/>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
     </row>
-    <row r="67" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C67" s="1"/>
       <c r="F67" s="1"/>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
     </row>
-    <row r="68" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C68" s="1"/>
       <c r="F68" s="1"/>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
     </row>
-    <row r="69" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C69" s="1"/>
       <c r="F69" s="1"/>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
     </row>
-    <row r="70" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C70" s="1"/>
       <c r="F70" s="1"/>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C71" s="1"/>
       <c r="F71" s="1"/>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C72" s="1"/>
       <c r="F72" s="1"/>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
-    <row r="73" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C73" s="1"/>
       <c r="F73" s="1"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
     </row>
-    <row r="74" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C74" s="1"/>
       <c r="F74" s="1"/>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
     </row>
-    <row r="75" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C75" s="1"/>
       <c r="F75" s="1"/>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
     </row>
-    <row r="76" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C76" s="1"/>
       <c r="F76" s="1"/>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
     </row>
-    <row r="77" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C77" s="1"/>
       <c r="F77" s="1"/>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
     </row>
-    <row r="78" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C78" s="1"/>
       <c r="F78" s="1"/>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
     </row>
-    <row r="79" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C79" s="1"/>
       <c r="F79" s="1"/>
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
-    <row r="80" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C80" s="1"/>
       <c r="F80" s="1"/>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
     </row>
-    <row r="81" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C81" s="1"/>
       <c r="F81" s="1"/>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
-    <row r="82" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C82" s="1"/>
       <c r="F82" s="1"/>
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
     </row>
-    <row r="83" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C83" s="1"/>
       <c r="F83" s="1"/>
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
     </row>
-    <row r="84" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C84" s="1"/>
       <c r="F84" s="1"/>
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
     </row>
-    <row r="85" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C85" s="1"/>
       <c r="F85" s="1"/>
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
     </row>
-    <row r="86" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C86" s="1"/>
       <c r="F86" s="1"/>
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
     </row>
-    <row r="87" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C87" s="1"/>
       <c r="F87" s="1"/>
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
     </row>
-    <row r="88" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C88" s="1"/>
       <c r="F88" s="1"/>
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
     </row>
-    <row r="89" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C89" s="1"/>
       <c r="F89" s="1"/>
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
     </row>
-    <row r="90" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C90" s="1"/>
       <c r="F90" s="1"/>
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
     </row>
-    <row r="91" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C91" s="1"/>
       <c r="F91" s="1"/>
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
     </row>
-    <row r="92" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C92" s="1"/>
       <c r="F92" s="1"/>
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
     </row>
-    <row r="93" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C93" s="1"/>
       <c r="F93" s="1"/>
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
     </row>
-    <row r="94" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C94" s="1"/>
       <c r="F94" s="1"/>
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
     </row>
-    <row r="95" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C95" s="1"/>
       <c r="F95" s="1"/>
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
     </row>
-    <row r="96" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C96" s="1"/>
       <c r="F96" s="1"/>
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
     </row>
-    <row r="97" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C97" s="1"/>
       <c r="F97" s="1"/>
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
     </row>
-    <row r="98" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C98" s="1"/>
       <c r="F98" s="1"/>
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
     </row>
-    <row r="99" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C99" s="1"/>
       <c r="F99" s="1"/>
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
     </row>
-    <row r="100" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C100" s="1"/>
       <c r="F100" s="1"/>
       <c r="H100" s="1"/>
@@ -1091,14 +1407,14 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.26953125" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B2">
@@ -1108,20 +1424,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <f>SUM('RL-GC data'!I2:I100)</f>
         <v>0</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="1">
@@ -1132,8 +1448,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="1">
@@ -1144,33 +1460,33 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <v>43842</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="8"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B9" s="7"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="9"/>
+      <c r="B10" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Improved Excel table for ETA calculation.
</commit_message>
<xml_diff>
--- a/matlab/voyage_plan.xlsx
+++ b/matlab/voyage_plan.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20820" windowHeight="13710"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20820" windowHeight="13710" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RL-GC data" sheetId="1" r:id="rId1"/>
     <sheet name="ETA calculator" sheetId="2" r:id="rId2"/>
+    <sheet name="Select Values" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
   <si>
     <t xml:space="preserve"> # </t>
   </si>
@@ -82,15 +83,67 @@
   </si>
   <si>
     <t xml:space="preserve"> [days]</t>
+  </si>
+  <si>
+    <t>Zone End</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Time zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [min]</t>
+  </si>
+  <si>
+    <t>Zone difference</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Longitude Start</t>
+  </si>
+  <si>
+    <t>Longitude End</t>
+  </si>
+  <si>
+    <t>Zone Start</t>
+  </si>
+  <si>
+    <t>deg</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>side</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
-    <numFmt numFmtId="165" formatCode="hh:mm:ss;@"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="hh:mm:ss;@"/>
+    <numFmt numFmtId="165" formatCode="dd\.mm\.yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -109,15 +162,45 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79995117038483843"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="34">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -202,6 +285,98 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -362,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -376,8 +551,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -389,14 +562,49 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -411,6 +619,29 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,7 +924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -709,285 +940,285 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2" s="1"/>
-      <c r="D2" s="30"/>
+      <c r="D2" s="41"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="30"/>
+      <c r="G2" s="41"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
-      <c r="D3" s="31"/>
+      <c r="D3" s="42"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="31"/>
+      <c r="G3" s="42"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
-      <c r="D4" s="32"/>
+      <c r="D4" s="43"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="32"/>
+      <c r="G4" s="43"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
-      <c r="D5" s="33"/>
+      <c r="D5" s="44"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="33"/>
+      <c r="G5" s="44"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
-      <c r="D6" s="34"/>
+      <c r="D6" s="45"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="34"/>
+      <c r="G6" s="45"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
-      <c r="D7" s="35"/>
+      <c r="D7" s="46"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="35"/>
+      <c r="G7" s="46"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
-      <c r="D8" s="36"/>
+      <c r="D8" s="47"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="36"/>
+      <c r="G8" s="47"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
-      <c r="D9" s="37"/>
+      <c r="D9" s="48"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="37"/>
+      <c r="G9" s="48"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
-      <c r="D10" s="38"/>
+      <c r="D10" s="49"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="38"/>
+      <c r="G10" s="49"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
-      <c r="D11" s="39"/>
+      <c r="D11" s="50"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="39"/>
+      <c r="G11" s="50"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
-      <c r="D12" s="40"/>
+      <c r="D12" s="51"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="40"/>
+      <c r="G12" s="51"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
-      <c r="D13" s="41"/>
+      <c r="D13" s="52"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="41"/>
+      <c r="G13" s="52"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
-      <c r="D14" s="10"/>
+      <c r="D14" s="53"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="10"/>
+      <c r="G14" s="53"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
-      <c r="D15" s="11"/>
+      <c r="D15" s="54"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="11"/>
+      <c r="G15" s="54"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
-      <c r="D16" s="12"/>
+      <c r="D16" s="55"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="12"/>
+      <c r="G16" s="55"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
-      <c r="D17" s="13"/>
+      <c r="D17" s="56"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="13"/>
+      <c r="G17" s="56"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
-      <c r="D18" s="14"/>
+      <c r="D18" s="57"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="14"/>
+      <c r="G18" s="57"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
-      <c r="D19" s="15"/>
+      <c r="D19" s="58"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="15"/>
+      <c r="G19" s="58"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
-      <c r="D20" s="16"/>
+      <c r="D20" s="59"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="16"/>
+      <c r="G20" s="59"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
-      <c r="D21" s="17"/>
+      <c r="D21" s="60"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="17"/>
+      <c r="G21" s="60"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
-      <c r="D22" s="18"/>
+      <c r="D22" s="61"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="18"/>
+      <c r="G22" s="61"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
-      <c r="D23" s="19"/>
+      <c r="D23" s="62"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="19"/>
+      <c r="G23" s="62"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
-      <c r="D24" s="20"/>
+      <c r="D24" s="8"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="20"/>
+      <c r="G24" s="8"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
-      <c r="D25" s="21"/>
+      <c r="D25" s="9"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="21"/>
+      <c r="G25" s="9"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
-      <c r="D26" s="22"/>
+      <c r="D26" s="10"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="22"/>
+      <c r="G26" s="10"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
-      <c r="D27" s="23"/>
+      <c r="D27" s="11"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="23"/>
+      <c r="G27" s="11"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
-      <c r="D28" s="24"/>
+      <c r="D28" s="12"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="24"/>
+      <c r="G28" s="12"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
-      <c r="D29" s="25"/>
+      <c r="D29" s="13"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="25"/>
+      <c r="G29" s="13"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
-      <c r="D30" s="26"/>
+      <c r="D30" s="14"/>
       <c r="F30" s="1"/>
-      <c r="G30" s="26"/>
+      <c r="G30" s="14"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C31" s="1"/>
-      <c r="D31" s="27"/>
+      <c r="D31" s="15"/>
       <c r="F31" s="1"/>
-      <c r="G31" s="27"/>
+      <c r="G31" s="15"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C32" s="1"/>
-      <c r="D32" s="28"/>
+      <c r="D32" s="16"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="28"/>
+      <c r="G32" s="16"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
-      <c r="D33" s="29"/>
+      <c r="D33" s="17"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="29"/>
+      <c r="G33" s="17"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
@@ -1401,19 +1632,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C10"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="3" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -1423,8 +1660,16 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="63" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="63"/>
+      <c r="H2" s="64" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="64"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -1435,58 +1680,244 @@
       <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="E3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="67">
+        <v>71</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="67">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="24">
         <f>B3/B2</f>
         <v>0</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="25" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="66">
+        <v>37</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="66">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1">
-        <f>B4/24</f>
+      <c r="B5" s="26">
+        <f>FLOOR(B4/24,1)</f>
         <v>0</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="E5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="26">
+        <f>FLOOR(B4-B5*24,1)</f>
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="28">
+        <f>FLOOR((B4-FLOOR(B4,1))*60,1)</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="1"/>
+      <c r="H8" s="18"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="7">
-        <v>43842</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B9" s="20">
+        <v>43907</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="38">
+        <f>F11*SIGN(F10)</f>
+        <v>-5</v>
+      </c>
+      <c r="G9" s="30"/>
+      <c r="H9" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="40">
+        <f>I11*SIGN(I10)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B10" s="36">
+        <v>0.53125</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="32">
+        <f>(F3 + F4/60)*IF(EXACT(F5,"W"),-1,1)</f>
+        <v>-71.61666666666666</v>
+      </c>
+      <c r="G10" s="30"/>
+      <c r="H10" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="32">
+        <f>(I3+I4/60)*IF(EXACT(I5,"W"),-1,1)</f>
+        <v>174.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="7"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B11" s="22">
+        <f>DATE(YEAR(B9),MONTH(B9),DAY(B9)+FLOOR(B5,1))</f>
+        <v>43907</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="6">
+        <f>FLOOR((ABS(F10)-7.5)/15,1)+1</f>
+        <v>5</v>
+      </c>
+      <c r="G11" s="30"/>
+      <c r="H11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="6">
+        <f>FLOOR((ABS(I10)-7.5)/15,1)+1</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B12" s="34">
+        <f>TIME(HOUR(B10)+B6+F13,MINUTE(B10)+B7,0)</f>
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="31">
+        <v>-7</v>
+      </c>
+      <c r="G13" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Select Values'!$B$2:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>F5 I5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="65" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="65" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="65" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>